<commit_message>
ImageRating Pictures now conditional with language
</commit_message>
<xml_diff>
--- a/Rating1.xlsx
+++ b/Rating1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329E019A-BBC4-874D-9C95-8D0F8446E863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5A802C-9E12-9642-81BF-202D7BBFE009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="2620" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="2660" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>TrgCol</t>
   </si>
   <si>
-    <t>ratingName</t>
-  </si>
-  <si>
     <t>Instructions_EN/ratingCS+1.png</t>
   </si>
   <si>
@@ -35,6 +32,21 @@
   </si>
   <si>
     <t>Instructions_EN/ratingCS+4.png</t>
+  </si>
+  <si>
+    <t>ratingName_EN</t>
+  </si>
+  <si>
+    <t>ratingName_CN</t>
+  </si>
+  <si>
+    <t>Instructions_CN/ratingCS+1.png</t>
+  </si>
+  <si>
+    <t>Instructions_CN/ratingCS+3.png</t>
+  </si>
+  <si>
+    <t>Instructions_CN/ratingCS+4.png</t>
   </si>
 </sst>
 </file>
@@ -382,47 +394,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="1" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5">
+        <v>-0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
-        <v>-0.1</v>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5">
         <v>-0.1</v>
       </c>
     </row>

</xml_diff>